<commit_message>
needed to correct table
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katxi\OneDrive\Mestrado\2nd Semester\Optimization\project\github\CI4O_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28DBA7FE-E49A-417D-B2D3-D254B6C3C0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA381A75-FAB1-4019-B6F9-6BFB8E2EC44E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{9DF1E2D6-5688-404C-8756-BC0ECA661880}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9DF1E2D6-5688-404C-8756-BC0ECA661880}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>Tournament Size</t>
   </si>
   <si>
-    <t>n/a</t>
-  </si>
-  <si>
     <t>Arithmetic Crossover</t>
   </si>
   <si>
@@ -84,6 +81,9 @@
   </si>
   <si>
     <t>Uniform Crossover</t>
+  </si>
+  <si>
+    <t>n.a.</t>
   </si>
 </sst>
 </file>
@@ -668,7 +668,7 @@
   <dimension ref="C2:H26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -706,7 +706,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>6</v>
@@ -718,7 +718,7 @@
         <v>7</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.3">
@@ -726,7 +726,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>6</v>
@@ -738,7 +738,7 @@
         <v>8</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.3">
@@ -746,10 +746,10 @@
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="F5" s="4">
         <v>0.9</v>
@@ -758,7 +758,7 @@
         <v>7</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.3">
@@ -766,10 +766,10 @@
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="F6" s="4">
         <v>0.9</v>
@@ -778,7 +778,7 @@
         <v>8</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.3">
@@ -786,19 +786,19 @@
         <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" s="4">
         <v>0.9</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.3">
@@ -806,10 +806,10 @@
         <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" s="4">
         <v>0.9</v>
@@ -818,15 +818,15 @@
         <v>8</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>6</v>
@@ -838,15 +838,15 @@
         <v>7</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>6</v>
@@ -858,18 +858,18 @@
         <v>8</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" s="4">
         <v>0.9</v>
@@ -878,18 +878,18 @@
         <v>7</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" s="4">
         <v>0.9</v>
@@ -898,18 +898,18 @@
         <v>8</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="F13" s="4">
         <v>0.9</v>
@@ -918,18 +918,18 @@
         <v>7</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C14" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>15</v>
       </c>
       <c r="F14" s="9">
         <v>0.9</v>
@@ -938,7 +938,7 @@
         <v>8</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.3">

</xml_diff>